<commit_message>
Enhance the ExcelExporter object
</commit_message>
<xml_diff>
--- a/server/classes/output.xlsx
+++ b/server/classes/output.xlsx
@@ -63,8 +63,8 @@
     <t>Hour Off Due</t>
   </si>
   <si>
-    <t xml:space="preserve">Resident Support
-Team Members</t>
+    <t xml:space="preserve">                              Date 
+Member .</t>
   </si>
   <si>
     <t>Last Month</t>
@@ -278,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -299,6 +299,15 @@
       <top style="thin"/>
       <bottom style="thin"/>
       <diagonal/>
+    </border>
+    <border diagonalDown="1">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="thin">
+        <color indexed="64"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -322,8 +331,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="distributed" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom"/>

</xml_diff>